<commit_message>
change diode + models
</commit_message>
<xml_diff>
--- a/BOM/Controls-MotorControllerBreakout.xlsx
+++ b/BOM/Controls-MotorControllerBreakout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi\Git\LHR\Controls-MotorControllerBreakout\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D54CFC34-4855-40FA-B6C7-CEA167E85988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252779D4-6B54-4E07-B899-CD072F8FC8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{61E53FAE-896E-4AEB-A3E3-0AE3A74F02CD}"/>
   </bookViews>
@@ -46,12 +46,6 @@
     <t>D2</t>
   </si>
   <si>
-    <t>1N4007</t>
-  </si>
-  <si>
-    <t>1N4007FL</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -110,6 +104,12 @@
   </si>
   <si>
     <t>CRCW080522K1FKEA</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>RS1MWF-7</t>
   </si>
 </sst>
 </file>
@@ -976,7 +976,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1018,35 +1018,35 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1057,10 +1057,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1071,10 +1071,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1085,10 +1085,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>120</v>
@@ -1130,21 +1130,21 @@
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hi its me again
</commit_message>
<xml_diff>
--- a/BOM/Controls-MotorControllerBreakout.xlsx
+++ b/BOM/Controls-MotorControllerBreakout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ravi\Git\LHR\Controls-MotorControllerBreakout\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8479983-43EE-4A86-BC31-5C864574B840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E075A99D-C92D-4033-9EEC-7C64BA7A6A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19543" windowHeight="12377" xr2:uid="{7B401F33-D8C4-476C-B06C-D44945A5EFE5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
   <si>
     <t>Reference</t>
   </si>
@@ -194,6 +194,12 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>D6,D7</t>
+  </si>
+  <si>
+    <t>VSSAF522-M3/H</t>
   </si>
 </sst>
 </file>
@@ -682,9 +688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1060,10 +1064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA640DE-B2BC-4F76-B987-64FD6990E339}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1078,13 +1082,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1092,13 +1096,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1106,13 +1110,13 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1120,13 +1124,13 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1134,13 +1138,13 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1148,248 +1152,263 @@
       <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>52</v>
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>430450612</v>
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>430450612</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>31</v>
+      <c r="D14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="1">
-        <v>120</v>
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>33</v>
+      <c r="D15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>120</v>
       </c>
       <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
       </c>
       <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
       </c>
       <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
       </c>
       <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>43</v>
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
+      <c r="D22" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" t="s">
         <v>50</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D24" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>